<commit_message>
changed "." to "NA"
</commit_message>
<xml_diff>
--- a/data/human_chr21.xlsx
+++ b/data/human_chr21.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="18420" yWindow="7480" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="human_chr21.txt" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <t>chr21</t>
   </si>
   <si>
-    <t>.</t>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -395,7 +395,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>

</xml_diff>